<commit_message>
Working on Boxer branches.
</commit_message>
<xml_diff>
--- a/spreadsheet/Hollard Branch List (All) 20170805 1050.xlsx
+++ b/spreadsheet/Hollard Branch List (All) 20170805 1050.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" tabRatio="599" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" tabRatio="599" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Retail Branch Boxer" sheetId="2" r:id="rId1"/>
     <sheet name="Hollard Branches" sheetId="6" r:id="rId2"/>
     <sheet name="Boxer Retail Branch" sheetId="7" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="386">
   <si>
     <t>Branch name</t>
   </si>
@@ -1170,6 +1170,15 @@
   </si>
   <si>
     <t>Uitval</t>
+  </si>
+  <si>
+    <t>GERT</t>
+  </si>
+  <si>
+    <t>VICTOR</t>
+  </si>
+  <si>
+    <t>MICHELLE</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1263,6 +1272,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1449,7 +1488,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1523,15 +1562,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1806,7 +1857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1816,9 +1867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2144,19 +2193,16 @@
   <dimension ref="A1:R133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="111.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.140625" customWidth="1"/>
-    <col min="16" max="18" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2186,17 +2232,19 @@
       <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
@@ -2212,17 +2260,19 @@
       <c r="R2" s="21"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
@@ -2238,17 +2288,19 @@
       <c r="R3" s="21"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
@@ -2264,17 +2316,19 @@
       <c r="R4" s="21"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
@@ -2290,17 +2344,19 @@
       <c r="R5" s="21"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="36" t="s">
         <v>203</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36" t="s">
         <v>203</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
@@ -2316,17 +2372,19 @@
       <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
@@ -2342,17 +2400,19 @@
       <c r="R7" s="21"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
@@ -2368,17 +2428,19 @@
       <c r="R8" s="21"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="37" t="s">
         <v>360</v>
       </c>
-      <c r="E9" s="34"/>
+      <c r="E9" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
@@ -2394,17 +2456,19 @@
       <c r="R9" s="21"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32" t="s">
+      <c r="B10" s="36"/>
+      <c r="C10" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -2420,17 +2484,19 @@
       <c r="R10" s="21"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38" t="s">
         <v>362</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="E11" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -2446,17 +2512,19 @@
       <c r="R11" s="21"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="E12" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
@@ -2472,17 +2540,19 @@
       <c r="R12" s="21"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32" t="s">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="34"/>
+      <c r="E13" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
@@ -2498,17 +2568,19 @@
       <c r="R13" s="21"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
@@ -2524,17 +2596,19 @@
       <c r="R14" s="21"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32" t="s">
+      <c r="B15" s="38"/>
+      <c r="C15" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
@@ -2550,17 +2624,19 @@
       <c r="R15" s="21"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32" t="s">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="E16" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
@@ -2576,17 +2652,19 @@
       <c r="R16" s="21"/>
     </row>
     <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32" t="s">
+      <c r="B17" s="38"/>
+      <c r="C17" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
@@ -2602,17 +2680,19 @@
       <c r="R17" s="21"/>
     </row>
     <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="E18" s="34"/>
+      <c r="E18" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
@@ -2628,17 +2708,19 @@
       <c r="R18" s="21"/>
     </row>
     <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="34"/>
+      <c r="E19" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F19" s="34"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
@@ -2654,17 +2736,19 @@
       <c r="R19" s="21"/>
     </row>
     <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
@@ -2680,17 +2764,19 @@
       <c r="R20" s="21"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="35" t="s">
+      <c r="B21" s="38"/>
+      <c r="C21" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="E21" s="34"/>
+      <c r="E21" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
@@ -2706,17 +2792,19 @@
       <c r="R21" s="21"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32" t="s">
+      <c r="B22" s="38"/>
+      <c r="C22" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="E22" s="34"/>
+      <c r="E22" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
       <c r="H22" s="34"/>
@@ -2732,17 +2820,19 @@
       <c r="R22" s="21"/>
     </row>
     <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="35" t="s">
+      <c r="B23" s="38"/>
+      <c r="C23" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="E23" s="34"/>
+      <c r="E23" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
@@ -2758,17 +2848,19 @@
       <c r="R23" s="21"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32" t="s">
+      <c r="B24" s="38"/>
+      <c r="C24" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="E24" s="34"/>
+      <c r="E24" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F24" s="34"/>
       <c r="G24" s="34"/>
       <c r="H24" s="34"/>
@@ -2784,17 +2876,19 @@
       <c r="R24" s="21"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32" t="s">
+      <c r="B25" s="38"/>
+      <c r="C25" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="E25" s="34"/>
+      <c r="E25" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F25" s="34"/>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
@@ -2810,17 +2904,19 @@
       <c r="R25" s="21"/>
     </row>
     <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32" t="s">
+      <c r="B26" s="38"/>
+      <c r="C26" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="34"/>
+      <c r="E26" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F26" s="34"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
@@ -2836,17 +2932,19 @@
       <c r="R26" s="21"/>
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32" t="s">
+      <c r="B27" s="38"/>
+      <c r="C27" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="34"/>
+      <c r="E27" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
@@ -2862,17 +2960,19 @@
       <c r="R27" s="21"/>
     </row>
     <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32" t="s">
+      <c r="B28" s="38"/>
+      <c r="C28" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="39" t="s">
         <v>335</v>
       </c>
-      <c r="E28" s="34"/>
+      <c r="E28" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
@@ -2888,17 +2988,19 @@
       <c r="R28" s="21"/>
     </row>
     <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32" t="s">
+      <c r="B29" s="38"/>
+      <c r="C29" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="39" t="s">
         <v>207</v>
       </c>
-      <c r="E29" s="34"/>
+      <c r="E29" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F29" s="34"/>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
@@ -2914,17 +3016,19 @@
       <c r="R29" s="21"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32" t="s">
+      <c r="B30" s="38"/>
+      <c r="C30" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="39" t="s">
         <v>248</v>
       </c>
-      <c r="E30" s="34"/>
+      <c r="E30" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F30" s="34"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
@@ -2940,17 +3044,19 @@
       <c r="R30" s="21"/>
     </row>
     <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32" t="s">
+      <c r="B31" s="38"/>
+      <c r="C31" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="E31" s="34"/>
+      <c r="E31" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F31" s="34"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
@@ -2966,17 +3072,19 @@
       <c r="R31" s="21"/>
     </row>
     <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32" t="s">
+      <c r="B32" s="38"/>
+      <c r="C32" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="E32" s="34"/>
+      <c r="E32" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F32" s="34"/>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
@@ -2992,17 +3100,19 @@
       <c r="R32" s="21"/>
     </row>
     <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32" t="s">
+      <c r="B33" s="38"/>
+      <c r="C33" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="39" t="s">
         <v>251</v>
       </c>
-      <c r="E33" s="34"/>
+      <c r="E33" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F33" s="34"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
@@ -3018,17 +3128,19 @@
       <c r="R33" s="21"/>
     </row>
     <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32" t="s">
+      <c r="B34" s="38"/>
+      <c r="C34" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="34"/>
+      <c r="E34" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F34" s="34"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
@@ -3044,17 +3156,19 @@
       <c r="R34" s="21"/>
     </row>
     <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32" t="s">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="34"/>
+      <c r="E35" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F35" s="34"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
@@ -3070,17 +3184,19 @@
       <c r="R35" s="21"/>
     </row>
     <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32" t="s">
+      <c r="B36" s="38"/>
+      <c r="C36" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="E36" s="34"/>
+      <c r="E36" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F36" s="34"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
@@ -3096,17 +3212,19 @@
       <c r="R36" s="21"/>
     </row>
     <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32" t="s">
+      <c r="B37" s="38"/>
+      <c r="C37" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="34"/>
+      <c r="E37" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F37" s="34"/>
       <c r="G37" s="34"/>
       <c r="H37" s="34"/>
@@ -3122,17 +3240,19 @@
       <c r="R37" s="21"/>
     </row>
     <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32" t="s">
+      <c r="B38" s="38"/>
+      <c r="C38" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="E38" s="34"/>
+      <c r="E38" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F38" s="34"/>
       <c r="G38" s="34"/>
       <c r="H38" s="34"/>
@@ -3148,17 +3268,19 @@
       <c r="R38" s="21"/>
     </row>
     <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32" t="s">
+      <c r="B39" s="38"/>
+      <c r="C39" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="34"/>
+      <c r="E39" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F39" s="34"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
@@ -3174,17 +3296,19 @@
       <c r="R39" s="21"/>
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32" t="s">
+      <c r="B40" s="38"/>
+      <c r="C40" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="34"/>
+      <c r="E40" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F40" s="34"/>
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
@@ -3200,17 +3324,19 @@
       <c r="R40" s="21"/>
     </row>
     <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="35" t="s">
+      <c r="B41" s="38"/>
+      <c r="C41" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="E41" s="34"/>
+      <c r="E41" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F41" s="34"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
@@ -3226,17 +3352,19 @@
       <c r="R41" s="21"/>
     </row>
     <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="35" t="s">
+      <c r="B42" s="38"/>
+      <c r="C42" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="E42" s="34"/>
+      <c r="E42" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
@@ -3252,17 +3380,19 @@
       <c r="R42" s="21"/>
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32" t="s">
+      <c r="B43" s="38"/>
+      <c r="C43" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="E43" s="34"/>
+      <c r="E43" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F43" s="34"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
@@ -3278,17 +3408,19 @@
       <c r="R43" s="21"/>
     </row>
     <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32" t="s">
+      <c r="B44" s="38"/>
+      <c r="C44" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="39" t="s">
         <v>336</v>
       </c>
-      <c r="E44" s="34"/>
+      <c r="E44" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F44" s="34"/>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
@@ -3304,17 +3436,19 @@
       <c r="R44" s="21"/>
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32" t="s">
+      <c r="B45" s="38"/>
+      <c r="C45" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="D45" s="34" t="s">
+      <c r="D45" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="E45" s="34"/>
+      <c r="E45" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F45" s="34"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
@@ -3330,17 +3464,19 @@
       <c r="R45" s="21"/>
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32" t="s">
+      <c r="B46" s="38"/>
+      <c r="C46" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="E46" s="34"/>
+      <c r="E46" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F46" s="34"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
@@ -3356,17 +3492,19 @@
       <c r="R46" s="21"/>
     </row>
     <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32" t="s">
+      <c r="B47" s="38"/>
+      <c r="C47" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="34" t="s">
+      <c r="D47" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="34"/>
+      <c r="E47" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F47" s="34"/>
       <c r="G47" s="34"/>
       <c r="H47" s="34"/>
@@ -3382,17 +3520,19 @@
       <c r="R47" s="21"/>
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32" t="s">
+      <c r="B48" s="38"/>
+      <c r="C48" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="E48" s="34"/>
+      <c r="E48" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F48" s="34"/>
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
@@ -3408,17 +3548,19 @@
       <c r="R48" s="21"/>
     </row>
     <row r="49" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32" t="s">
+      <c r="B49" s="38"/>
+      <c r="C49" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="E49" s="34"/>
+      <c r="E49" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F49" s="34"/>
       <c r="G49" s="34"/>
       <c r="H49" s="34"/>
@@ -3434,17 +3576,19 @@
       <c r="R49" s="21"/>
     </row>
     <row r="50" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32" t="s">
+      <c r="B50" s="38"/>
+      <c r="C50" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="E50" s="34"/>
+      <c r="E50" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F50" s="34"/>
       <c r="G50" s="34"/>
       <c r="H50" s="34"/>
@@ -3460,17 +3604,19 @@
       <c r="R50" s="21"/>
     </row>
     <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32" t="s">
+      <c r="B51" s="38"/>
+      <c r="C51" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="D51" s="34" t="s">
+      <c r="D51" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="E51" s="34"/>
+      <c r="E51" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F51" s="34"/>
       <c r="G51" s="34"/>
       <c r="H51" s="34"/>
@@ -3486,17 +3632,19 @@
       <c r="R51" s="21"/>
     </row>
     <row r="52" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="32" t="s">
+      <c r="A52" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="B52" s="32"/>
-      <c r="C52" s="36" t="s">
+      <c r="B52" s="38"/>
+      <c r="C52" s="41" t="s">
         <v>351</v>
       </c>
-      <c r="D52" s="34" t="s">
+      <c r="D52" s="39" t="s">
         <v>337</v>
       </c>
-      <c r="E52" s="34"/>
+      <c r="E52" s="34" t="s">
+        <v>384</v>
+      </c>
       <c r="F52" s="34"/>
       <c r="G52" s="34"/>
       <c r="H52" s="34"/>
@@ -3512,17 +3660,19 @@
       <c r="R52" s="21"/>
     </row>
     <row r="53" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32" t="s">
+      <c r="B53" s="42"/>
+      <c r="C53" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="D53" s="34" t="s">
+      <c r="D53" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="E53" s="34"/>
+      <c r="E53" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F53" s="34"/>
       <c r="G53" s="34"/>
       <c r="H53" s="34"/>
@@ -3538,17 +3688,19 @@
       <c r="R53" s="21"/>
     </row>
     <row r="54" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="32" t="s">
+      <c r="A54" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32" t="s">
+      <c r="B54" s="42"/>
+      <c r="C54" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="34" t="s">
+      <c r="D54" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="E54" s="34"/>
+      <c r="E54" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F54" s="34"/>
       <c r="G54" s="34"/>
       <c r="H54" s="34"/>
@@ -3564,17 +3716,19 @@
       <c r="R54" s="21"/>
     </row>
     <row r="55" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="32" t="s">
+      <c r="A55" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32" t="s">
+      <c r="B55" s="42"/>
+      <c r="C55" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="D55" s="34" t="s">
+      <c r="D55" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="E55" s="34"/>
+      <c r="E55" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F55" s="34"/>
       <c r="G55" s="34"/>
       <c r="H55" s="34"/>
@@ -3590,17 +3744,19 @@
       <c r="R55" s="21"/>
     </row>
     <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
+      <c r="A56" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32" t="s">
+      <c r="B56" s="42"/>
+      <c r="C56" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D56" s="34" t="s">
+      <c r="D56" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E56" s="34"/>
+      <c r="E56" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F56" s="34"/>
       <c r="G56" s="34"/>
       <c r="H56" s="34"/>
@@ -3616,17 +3772,19 @@
       <c r="R56" s="21"/>
     </row>
     <row r="57" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="32" t="s">
+      <c r="A57" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="32"/>
-      <c r="C57" s="32" t="s">
+      <c r="B57" s="42"/>
+      <c r="C57" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D57" s="34" t="s">
+      <c r="D57" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="E57" s="34"/>
+      <c r="E57" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F57" s="34"/>
       <c r="G57" s="34"/>
       <c r="H57" s="34"/>
@@ -3642,17 +3800,19 @@
       <c r="R57" s="21"/>
     </row>
     <row r="58" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="32" t="s">
+      <c r="A58" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="32" t="s">
+      <c r="B58" s="42"/>
+      <c r="C58" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="D58" s="34" t="s">
+      <c r="D58" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="E58" s="34"/>
+      <c r="E58" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F58" s="34"/>
       <c r="G58" s="34"/>
       <c r="H58" s="34"/>
@@ -3668,17 +3828,19 @@
       <c r="R58" s="21"/>
     </row>
     <row r="59" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="32"/>
-      <c r="C59" s="32" t="s">
+      <c r="B59" s="42"/>
+      <c r="C59" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E59" s="34"/>
+      <c r="E59" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F59" s="34"/>
       <c r="G59" s="34"/>
       <c r="H59" s="34"/>
@@ -3694,17 +3856,19 @@
       <c r="R59" s="21"/>
     </row>
     <row r="60" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="32" t="s">
+      <c r="A60" s="42" t="s">
         <v>323</v>
       </c>
-      <c r="B60" s="32"/>
-      <c r="C60" s="32" t="s">
+      <c r="B60" s="42"/>
+      <c r="C60" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="D60" s="34" t="s">
+      <c r="D60" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="E60" s="34"/>
+      <c r="E60" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F60" s="34"/>
       <c r="G60" s="34"/>
       <c r="H60" s="34"/>
@@ -3720,17 +3884,19 @@
       <c r="R60" s="21"/>
     </row>
     <row r="61" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="32" t="s">
+      <c r="A61" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32" t="s">
+      <c r="B61" s="42"/>
+      <c r="C61" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="D61" s="34" t="s">
+      <c r="D61" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="E61" s="34"/>
+      <c r="E61" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F61" s="34"/>
       <c r="G61" s="34"/>
       <c r="H61" s="34"/>
@@ -3746,17 +3912,19 @@
       <c r="R61" s="21"/>
     </row>
     <row r="62" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="32" t="s">
+      <c r="A62" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32" t="s">
+      <c r="B62" s="42"/>
+      <c r="C62" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="D62" s="34" t="s">
+      <c r="D62" s="43" t="s">
         <v>338</v>
       </c>
-      <c r="E62" s="34"/>
+      <c r="E62" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F62" s="34"/>
       <c r="G62" s="34"/>
       <c r="H62" s="34"/>
@@ -3772,17 +3940,19 @@
       <c r="R62" s="21"/>
     </row>
     <row r="63" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
+      <c r="A63" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32" t="s">
+      <c r="B63" s="42"/>
+      <c r="C63" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="D63" s="34" t="s">
+      <c r="D63" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="E63" s="34"/>
+      <c r="E63" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F63" s="34"/>
       <c r="G63" s="34"/>
       <c r="H63" s="34"/>
@@ -3798,17 +3968,19 @@
       <c r="R63" s="21"/>
     </row>
     <row r="64" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="32" t="s">
+      <c r="A64" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="B64" s="32"/>
-      <c r="C64" s="35" t="s">
+      <c r="B64" s="42"/>
+      <c r="C64" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="34" t="s">
+      <c r="D64" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="E64" s="34"/>
+      <c r="E64" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F64" s="34"/>
       <c r="G64" s="34"/>
       <c r="H64" s="34"/>
@@ -3824,17 +3996,19 @@
       <c r="R64" s="21"/>
     </row>
     <row r="65" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="32" t="s">
+      <c r="A65" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="B65" s="32"/>
-      <c r="C65" s="32" t="s">
+      <c r="B65" s="42"/>
+      <c r="C65" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D65" s="34" t="s">
+      <c r="D65" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="E65" s="34"/>
+      <c r="E65" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F65" s="34"/>
       <c r="G65" s="34"/>
       <c r="H65" s="34"/>
@@ -3850,17 +4024,19 @@
       <c r="R65" s="21"/>
     </row>
     <row r="66" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="32" t="s">
+      <c r="A66" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B66" s="32"/>
-      <c r="C66" s="32" t="s">
+      <c r="B66" s="42"/>
+      <c r="C66" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D66" s="34" t="s">
+      <c r="D66" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="E66" s="34"/>
+      <c r="E66" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F66" s="34"/>
       <c r="G66" s="34"/>
       <c r="H66" s="34"/>
@@ -3876,17 +4052,19 @@
       <c r="R66" s="21"/>
     </row>
     <row r="67" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="32" t="s">
+      <c r="A67" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32" t="s">
+      <c r="B67" s="42"/>
+      <c r="C67" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="34" t="s">
+      <c r="D67" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="E67" s="34"/>
+      <c r="E67" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F67" s="34"/>
       <c r="G67" s="34"/>
       <c r="H67" s="34"/>
@@ -3902,17 +4080,19 @@
       <c r="R67" s="21"/>
     </row>
     <row r="68" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="32" t="s">
+      <c r="A68" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="B68" s="32"/>
-      <c r="C68" s="32" t="s">
+      <c r="B68" s="42"/>
+      <c r="C68" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="D68" s="34" t="s">
+      <c r="D68" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="E68" s="34"/>
+      <c r="E68" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F68" s="34"/>
       <c r="G68" s="34"/>
       <c r="H68" s="34"/>
@@ -3928,17 +4108,19 @@
       <c r="R68" s="21"/>
     </row>
     <row r="69" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32" t="s">
+      <c r="B69" s="42"/>
+      <c r="C69" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D69" s="34" t="s">
+      <c r="D69" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E69" s="34"/>
+      <c r="E69" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F69" s="34"/>
       <c r="G69" s="34"/>
       <c r="H69" s="34"/>
@@ -3954,17 +4136,19 @@
       <c r="R69" s="21"/>
     </row>
     <row r="70" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="32" t="s">
+      <c r="A70" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="B70" s="32"/>
-      <c r="C70" s="32" t="s">
+      <c r="B70" s="42"/>
+      <c r="C70" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="D70" s="34" t="s">
+      <c r="D70" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="E70" s="34"/>
+      <c r="E70" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F70" s="34"/>
       <c r="G70" s="34"/>
       <c r="H70" s="34"/>
@@ -3980,17 +4164,19 @@
       <c r="R70" s="21"/>
     </row>
     <row r="71" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="32" t="s">
+      <c r="A71" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="B71" s="32"/>
-      <c r="C71" s="32" t="s">
+      <c r="B71" s="42"/>
+      <c r="C71" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="D71" s="34" t="s">
+      <c r="D71" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="E71" s="34"/>
+      <c r="E71" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F71" s="34"/>
       <c r="G71" s="34"/>
       <c r="H71" s="34"/>
@@ -4006,17 +4192,19 @@
       <c r="R71" s="21"/>
     </row>
     <row r="72" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="32" t="s">
+      <c r="A72" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="B72" s="32"/>
-      <c r="C72" s="35" t="s">
+      <c r="B72" s="42"/>
+      <c r="C72" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="D72" s="34" t="s">
+      <c r="D72" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="E72" s="34"/>
+      <c r="E72" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F72" s="34"/>
       <c r="G72" s="34"/>
       <c r="H72" s="34"/>
@@ -4032,17 +4220,19 @@
       <c r="R72" s="21"/>
     </row>
     <row r="73" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="32" t="s">
+      <c r="A73" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="B73" s="32"/>
-      <c r="C73" s="35" t="s">
+      <c r="B73" s="42"/>
+      <c r="C73" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="D73" s="34" t="s">
+      <c r="D73" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="E73" s="34"/>
+      <c r="E73" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F73" s="34"/>
       <c r="G73" s="34"/>
       <c r="H73" s="34"/>
@@ -4058,17 +4248,19 @@
       <c r="R73" s="21"/>
     </row>
     <row r="74" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="32" t="s">
+      <c r="A74" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32" t="s">
+      <c r="B74" s="42"/>
+      <c r="C74" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D74" s="34" t="s">
+      <c r="D74" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E74" s="34"/>
+      <c r="E74" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F74" s="34"/>
       <c r="G74" s="34"/>
       <c r="H74" s="34"/>
@@ -4084,17 +4276,19 @@
       <c r="R74" s="21"/>
     </row>
     <row r="75" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="32" t="s">
+      <c r="A75" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="B75" s="32"/>
-      <c r="C75" s="35" t="s">
+      <c r="B75" s="42"/>
+      <c r="C75" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="D75" s="34" t="s">
+      <c r="D75" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="E75" s="34"/>
+      <c r="E75" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F75" s="34"/>
       <c r="G75" s="34"/>
       <c r="H75" s="34"/>
@@ -4110,17 +4304,19 @@
       <c r="R75" s="21"/>
     </row>
     <row r="76" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="32" t="s">
+      <c r="A76" s="42" t="s">
         <v>254</v>
       </c>
-      <c r="B76" s="32"/>
-      <c r="C76" s="32" t="s">
+      <c r="B76" s="42"/>
+      <c r="C76" s="42" t="s">
         <v>254</v>
       </c>
-      <c r="D76" s="34" t="s">
+      <c r="D76" s="43" t="s">
         <v>255</v>
       </c>
-      <c r="E76" s="34"/>
+      <c r="E76" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F76" s="34"/>
       <c r="G76" s="34"/>
       <c r="H76" s="34"/>
@@ -4136,17 +4332,19 @@
       <c r="R76" s="21"/>
     </row>
     <row r="77" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="32" t="s">
+      <c r="A77" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B77" s="32"/>
-      <c r="C77" s="32" t="s">
+      <c r="B77" s="42"/>
+      <c r="C77" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="34" t="s">
+      <c r="D77" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E77" s="34"/>
+      <c r="E77" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F77" s="34"/>
       <c r="G77" s="34"/>
       <c r="H77" s="34"/>
@@ -4162,17 +4360,19 @@
       <c r="R77" s="21"/>
     </row>
     <row r="78" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="32" t="s">
+      <c r="A78" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B78" s="32"/>
-      <c r="C78" s="32" t="s">
+      <c r="B78" s="42"/>
+      <c r="C78" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D78" s="34" t="s">
+      <c r="D78" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="E78" s="34"/>
+      <c r="E78" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F78" s="34"/>
       <c r="G78" s="34"/>
       <c r="H78" s="34"/>
@@ -4188,17 +4388,19 @@
       <c r="R78" s="21"/>
     </row>
     <row r="79" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="32" t="s">
+      <c r="A79" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32" t="s">
+      <c r="B79" s="42"/>
+      <c r="C79" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="D79" s="34" t="s">
+      <c r="D79" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="E79" s="34"/>
+      <c r="E79" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F79" s="34"/>
       <c r="G79" s="34"/>
       <c r="H79" s="34"/>
@@ -4214,17 +4416,19 @@
       <c r="R79" s="21"/>
     </row>
     <row r="80" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="32" t="s">
+      <c r="A80" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B80" s="32"/>
-      <c r="C80" s="32" t="s">
+      <c r="B80" s="42"/>
+      <c r="C80" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="34" t="s">
+      <c r="D80" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E80" s="34"/>
+      <c r="E80" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F80" s="34"/>
       <c r="G80" s="34"/>
       <c r="H80" s="34"/>
@@ -4240,17 +4444,19 @@
       <c r="R80" s="21"/>
     </row>
     <row r="81" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="32" t="s">
+      <c r="A81" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="B81" s="32"/>
-      <c r="C81" s="32" t="s">
+      <c r="B81" s="42"/>
+      <c r="C81" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="D81" s="34" t="s">
+      <c r="D81" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="E81" s="34"/>
+      <c r="E81" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F81" s="34"/>
       <c r="G81" s="34"/>
       <c r="H81" s="34"/>
@@ -4266,17 +4472,19 @@
       <c r="R81" s="21"/>
     </row>
     <row r="82" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="32" t="s">
+      <c r="A82" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="B82" s="32"/>
-      <c r="C82" s="32" t="s">
+      <c r="B82" s="42"/>
+      <c r="C82" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D82" s="34" t="s">
+      <c r="D82" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="E82" s="34"/>
+      <c r="E82" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F82" s="34"/>
       <c r="G82" s="34"/>
       <c r="H82" s="34"/>
@@ -4292,17 +4500,19 @@
       <c r="R82" s="21"/>
     </row>
     <row r="83" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="32" t="s">
+      <c r="A83" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="32"/>
-      <c r="C83" s="32" t="s">
+      <c r="B83" s="42"/>
+      <c r="C83" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="D83" s="34" t="s">
+      <c r="D83" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="E83" s="34"/>
+      <c r="E83" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F83" s="34"/>
       <c r="G83" s="34"/>
       <c r="H83" s="34"/>
@@ -4318,17 +4528,19 @@
       <c r="R83" s="21"/>
     </row>
     <row r="84" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="32" t="s">
+      <c r="A84" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32" t="s">
+      <c r="B84" s="42"/>
+      <c r="C84" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D84" s="34" t="s">
+      <c r="D84" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="E84" s="34"/>
+      <c r="E84" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F84" s="34"/>
       <c r="G84" s="34"/>
       <c r="H84" s="34"/>
@@ -4344,17 +4556,19 @@
       <c r="R84" s="21"/>
     </row>
     <row r="85" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="32" t="s">
+      <c r="A85" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32" t="s">
+      <c r="B85" s="42"/>
+      <c r="C85" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D85" s="34" t="s">
+      <c r="D85" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E85" s="34"/>
+      <c r="E85" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F85" s="34"/>
       <c r="G85" s="34"/>
       <c r="H85" s="34"/>
@@ -4370,17 +4584,19 @@
       <c r="R85" s="21"/>
     </row>
     <row r="86" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="32" t="s">
+      <c r="A86" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32" t="s">
+      <c r="B86" s="42"/>
+      <c r="C86" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D86" s="34" t="s">
+      <c r="D86" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E86" s="34"/>
+      <c r="E86" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F86" s="34"/>
       <c r="G86" s="34"/>
       <c r="H86" s="34"/>
@@ -4396,17 +4612,19 @@
       <c r="R86" s="21"/>
     </row>
     <row r="87" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="32" t="s">
+      <c r="A87" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="B87" s="32"/>
-      <c r="C87" s="32" t="s">
+      <c r="B87" s="42"/>
+      <c r="C87" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="D87" s="34" t="s">
+      <c r="D87" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="E87" s="34"/>
+      <c r="E87" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F87" s="34"/>
       <c r="G87" s="34"/>
       <c r="H87" s="34"/>
@@ -4422,17 +4640,19 @@
       <c r="R87" s="21"/>
     </row>
     <row r="88" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="32" t="s">
+      <c r="A88" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="B88" s="32"/>
-      <c r="C88" s="32" t="s">
+      <c r="B88" s="42"/>
+      <c r="C88" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="D88" s="34" t="s">
+      <c r="D88" s="43" t="s">
         <v>339</v>
       </c>
-      <c r="E88" s="34"/>
+      <c r="E88" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F88" s="34"/>
       <c r="G88" s="34"/>
       <c r="H88" s="34"/>
@@ -4448,17 +4668,19 @@
       <c r="R88" s="21"/>
     </row>
     <row r="89" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="32" t="s">
+      <c r="A89" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="B89" s="32"/>
-      <c r="C89" s="32" t="s">
+      <c r="B89" s="42"/>
+      <c r="C89" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="D89" s="34" t="s">
+      <c r="D89" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="E89" s="34"/>
+      <c r="E89" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F89" s="34"/>
       <c r="G89" s="34"/>
       <c r="H89" s="34"/>
@@ -4474,17 +4696,19 @@
       <c r="R89" s="21"/>
     </row>
     <row r="90" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="32" t="s">
+      <c r="A90" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="B90" s="32"/>
-      <c r="C90" s="32" t="s">
+      <c r="B90" s="42"/>
+      <c r="C90" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="D90" s="34" t="s">
+      <c r="D90" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="E90" s="34"/>
+      <c r="E90" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F90" s="34"/>
       <c r="G90" s="34"/>
       <c r="H90" s="34"/>
@@ -4500,17 +4724,19 @@
       <c r="R90" s="21"/>
     </row>
     <row r="91" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="32" t="s">
+      <c r="A91" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="B91" s="32"/>
-      <c r="C91" s="32" t="s">
+      <c r="B91" s="42"/>
+      <c r="C91" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="D91" s="34" t="s">
+      <c r="D91" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="E91" s="34"/>
+      <c r="E91" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F91" s="34"/>
       <c r="G91" s="34"/>
       <c r="H91" s="34"/>
@@ -4526,17 +4752,19 @@
       <c r="R91" s="21"/>
     </row>
     <row r="92" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="32" t="s">
+      <c r="A92" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="B92" s="32"/>
-      <c r="C92" s="32" t="s">
+      <c r="B92" s="42"/>
+      <c r="C92" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="D92" s="34" t="s">
+      <c r="D92" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="E92" s="34"/>
+      <c r="E92" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F92" s="34"/>
       <c r="G92" s="34"/>
       <c r="H92" s="34"/>
@@ -4552,17 +4780,19 @@
       <c r="R92" s="21"/>
     </row>
     <row r="93" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="32" t="s">
+      <c r="A93" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B93" s="32"/>
-      <c r="C93" s="32" t="s">
+      <c r="B93" s="42"/>
+      <c r="C93" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D93" s="34" t="s">
+      <c r="D93" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E93" s="34"/>
+      <c r="E93" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F93" s="34"/>
       <c r="G93" s="34"/>
       <c r="H93" s="34"/>
@@ -4578,17 +4808,19 @@
       <c r="R93" s="21"/>
     </row>
     <row r="94" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="32" t="s">
+      <c r="A94" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B94" s="32"/>
-      <c r="C94" s="32" t="s">
+      <c r="B94" s="42"/>
+      <c r="C94" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="D94" s="34" t="s">
+      <c r="D94" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="E94" s="34"/>
+      <c r="E94" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F94" s="34"/>
       <c r="G94" s="34"/>
       <c r="H94" s="34"/>
@@ -4604,17 +4836,19 @@
       <c r="R94" s="21"/>
     </row>
     <row r="95" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="32" t="s">
+      <c r="A95" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="B95" s="32"/>
-      <c r="C95" s="32" t="s">
+      <c r="B95" s="45"/>
+      <c r="C95" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="D95" s="34" t="s">
+      <c r="D95" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="E95" s="34"/>
+      <c r="E95" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F95" s="34"/>
       <c r="G95" s="34"/>
       <c r="H95" s="34"/>
@@ -4630,17 +4864,19 @@
       <c r="R95" s="21"/>
     </row>
     <row r="96" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="32" t="s">
+      <c r="A96" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="B96" s="32"/>
-      <c r="C96" s="32" t="s">
+      <c r="B96" s="45"/>
+      <c r="C96" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="D96" s="34" t="s">
+      <c r="D96" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="E96" s="34"/>
+      <c r="E96" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F96" s="34"/>
       <c r="G96" s="34"/>
       <c r="H96" s="34"/>
@@ -4656,17 +4892,19 @@
       <c r="R96" s="21"/>
     </row>
     <row r="97" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="32" t="s">
+      <c r="A97" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="B97" s="32"/>
-      <c r="C97" s="32" t="s">
+      <c r="B97" s="45"/>
+      <c r="C97" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="D97" s="34" t="s">
+      <c r="D97" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="E97" s="34"/>
+      <c r="E97" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F97" s="34"/>
       <c r="G97" s="34"/>
       <c r="H97" s="34"/>
@@ -4682,17 +4920,19 @@
       <c r="R97" s="21"/>
     </row>
     <row r="98" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="32" t="s">
+      <c r="A98" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="B98" s="32"/>
-      <c r="C98" s="32" t="s">
+      <c r="B98" s="45"/>
+      <c r="C98" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="D98" s="34" t="s">
+      <c r="D98" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="E98" s="34"/>
+      <c r="E98" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F98" s="34"/>
       <c r="G98" s="34"/>
       <c r="H98" s="34"/>
@@ -4708,17 +4948,19 @@
       <c r="R98" s="21"/>
     </row>
     <row r="99" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="32" t="s">
+      <c r="A99" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="B99" s="32"/>
-      <c r="C99" s="32" t="s">
+      <c r="B99" s="45"/>
+      <c r="C99" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="D99" s="34" t="s">
+      <c r="D99" s="46" t="s">
         <v>177</v>
       </c>
-      <c r="E99" s="34"/>
+      <c r="E99" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F99" s="34"/>
       <c r="G99" s="34"/>
       <c r="H99" s="34"/>
@@ -4734,17 +4976,19 @@
       <c r="R99" s="21"/>
     </row>
     <row r="100" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="32" t="s">
+      <c r="A100" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="B100" s="32"/>
-      <c r="C100" s="32" t="s">
+      <c r="B100" s="45"/>
+      <c r="C100" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="D100" s="37" t="s">
+      <c r="D100" s="45" t="s">
         <v>359</v>
       </c>
-      <c r="E100" s="34"/>
+      <c r="E100" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F100" s="34"/>
       <c r="G100" s="34"/>
       <c r="H100" s="34"/>
@@ -4760,17 +5004,19 @@
       <c r="R100" s="21"/>
     </row>
     <row r="101" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="32" t="s">
+      <c r="A101" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B101" s="32"/>
-      <c r="C101" s="32" t="s">
+      <c r="B101" s="45"/>
+      <c r="C101" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="D101" s="34" t="s">
+      <c r="D101" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="E101" s="34"/>
+      <c r="E101" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F101" s="34"/>
       <c r="G101" s="34"/>
       <c r="H101" s="34"/>
@@ -4786,17 +5032,19 @@
       <c r="R101" s="21"/>
     </row>
     <row r="102" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="32" t="s">
+      <c r="A102" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="B102" s="32"/>
-      <c r="C102" s="32" t="s">
+      <c r="B102" s="45"/>
+      <c r="C102" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="D102" s="34" t="s">
+      <c r="D102" s="46" t="s">
         <v>228</v>
       </c>
-      <c r="E102" s="34"/>
+      <c r="E102" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F102" s="34"/>
       <c r="G102" s="34"/>
       <c r="H102" s="34"/>
@@ -4812,17 +5060,19 @@
       <c r="R102" s="21"/>
     </row>
     <row r="103" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="32" t="s">
+      <c r="A103" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="B103" s="32"/>
-      <c r="C103" s="32" t="s">
+      <c r="B103" s="45"/>
+      <c r="C103" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D103" s="34" t="s">
+      <c r="D103" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="E103" s="34"/>
+      <c r="E103" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F103" s="34"/>
       <c r="G103" s="34"/>
       <c r="H103" s="34"/>
@@ -4838,17 +5088,19 @@
       <c r="R103" s="21"/>
     </row>
     <row r="104" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="32" t="s">
+      <c r="A104" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="B104" s="32"/>
-      <c r="C104" s="32" t="s">
+      <c r="B104" s="45"/>
+      <c r="C104" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="D104" s="34" t="s">
+      <c r="D104" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="E104" s="34"/>
+      <c r="E104" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F104" s="34"/>
       <c r="G104" s="34"/>
       <c r="H104" s="34"/>
@@ -4864,17 +5116,19 @@
       <c r="R104" s="21"/>
     </row>
     <row r="105" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="32" t="s">
+      <c r="A105" s="45" t="s">
         <v>354</v>
       </c>
-      <c r="B105" s="32"/>
-      <c r="C105" s="32" t="s">
+      <c r="B105" s="45"/>
+      <c r="C105" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="D105" s="34" t="s">
+      <c r="D105" s="46" t="s">
         <v>357</v>
       </c>
-      <c r="E105" s="34"/>
+      <c r="E105" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F105" s="34"/>
       <c r="G105" s="34"/>
       <c r="H105" s="34"/>
@@ -4890,17 +5144,19 @@
       <c r="R105" s="21"/>
     </row>
     <row r="106" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="32" t="s">
+      <c r="A106" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="B106" s="32"/>
-      <c r="C106" s="32" t="s">
+      <c r="B106" s="45"/>
+      <c r="C106" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="D106" s="34" t="s">
+      <c r="D106" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="E106" s="34"/>
+      <c r="E106" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F106" s="34"/>
       <c r="G106" s="34"/>
       <c r="H106" s="34"/>
@@ -4916,17 +5172,19 @@
       <c r="R106" s="21"/>
     </row>
     <row r="107" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="32" t="s">
+      <c r="A107" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="B107" s="32"/>
-      <c r="C107" s="32" t="s">
+      <c r="B107" s="45"/>
+      <c r="C107" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="D107" s="34" t="s">
+      <c r="D107" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="E107" s="34"/>
+      <c r="E107" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F107" s="34"/>
       <c r="G107" s="34"/>
       <c r="H107" s="34"/>
@@ -4942,17 +5200,19 @@
       <c r="R107" s="21"/>
     </row>
     <row r="108" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="32" t="s">
+      <c r="A108" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="B108" s="32"/>
-      <c r="C108" s="32" t="s">
+      <c r="B108" s="45"/>
+      <c r="C108" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="D108" s="34" t="s">
+      <c r="D108" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="E108" s="34"/>
+      <c r="E108" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F108" s="34"/>
       <c r="G108" s="34"/>
       <c r="H108" s="34"/>
@@ -4968,17 +5228,19 @@
       <c r="R108" s="21"/>
     </row>
     <row r="109" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="32" t="s">
+      <c r="A109" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B109" s="32"/>
-      <c r="C109" s="32" t="s">
+      <c r="B109" s="45"/>
+      <c r="C109" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D109" s="34" t="s">
+      <c r="D109" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="E109" s="34"/>
+      <c r="E109" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F109" s="34"/>
       <c r="G109" s="34"/>
       <c r="H109" s="34"/>
@@ -4994,17 +5256,19 @@
       <c r="R109" s="21"/>
     </row>
     <row r="110" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="32" t="s">
+      <c r="A110" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="B110" s="32"/>
-      <c r="C110" s="32" t="s">
+      <c r="B110" s="45"/>
+      <c r="C110" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="D110" s="34" t="s">
+      <c r="D110" s="46" t="s">
         <v>253</v>
       </c>
-      <c r="E110" s="34"/>
+      <c r="E110" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F110" s="34"/>
       <c r="G110" s="34"/>
       <c r="H110" s="34"/>
@@ -5020,17 +5284,19 @@
       <c r="R110" s="21"/>
     </row>
     <row r="111" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="32" t="s">
+      <c r="A111" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="B111" s="32"/>
-      <c r="C111" s="32" t="s">
+      <c r="B111" s="45"/>
+      <c r="C111" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="D111" s="34" t="s">
+      <c r="D111" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="E111" s="34"/>
+      <c r="E111" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F111" s="34"/>
       <c r="G111" s="34"/>
       <c r="H111" s="34"/>
@@ -5046,17 +5312,19 @@
       <c r="R111" s="21"/>
     </row>
     <row r="112" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="32" t="s">
+      <c r="A112" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="B112" s="32"/>
-      <c r="C112" s="32" t="s">
+      <c r="B112" s="45"/>
+      <c r="C112" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="D112" s="34" t="s">
+      <c r="D112" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="E112" s="34"/>
+      <c r="E112" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F112" s="34"/>
       <c r="G112" s="34"/>
       <c r="H112" s="34"/>
@@ -5072,17 +5340,19 @@
       <c r="R112" s="21"/>
     </row>
     <row r="113" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="32" t="s">
+      <c r="A113" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="B113" s="32"/>
-      <c r="C113" s="32" t="s">
+      <c r="B113" s="45"/>
+      <c r="C113" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="D113" s="34" t="s">
+      <c r="D113" s="46" t="s">
         <v>246</v>
       </c>
-      <c r="E113" s="34"/>
+      <c r="E113" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F113" s="34"/>
       <c r="G113" s="34"/>
       <c r="H113" s="34"/>
@@ -5098,17 +5368,19 @@
       <c r="R113" s="21"/>
     </row>
     <row r="114" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="32" t="s">
+      <c r="A114" s="45" t="s">
         <v>324</v>
       </c>
-      <c r="B114" s="32"/>
-      <c r="C114" s="32" t="s">
+      <c r="B114" s="45"/>
+      <c r="C114" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="D114" s="34" t="s">
+      <c r="D114" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="E114" s="34"/>
+      <c r="E114" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="F114" s="34"/>
       <c r="G114" s="34"/>
       <c r="H114" s="34"/>
@@ -5124,17 +5396,19 @@
       <c r="R114" s="21"/>
     </row>
     <row r="115" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="32" t="s">
+      <c r="A115" s="47" t="s">
         <v>258</v>
       </c>
-      <c r="B115" s="32"/>
-      <c r="C115" s="32" t="s">
+      <c r="B115" s="47"/>
+      <c r="C115" s="47" t="s">
         <v>258</v>
       </c>
-      <c r="D115" s="34" t="s">
+      <c r="D115" s="48" t="s">
         <v>259</v>
       </c>
-      <c r="E115" s="34"/>
+      <c r="E115" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F115" s="34"/>
       <c r="G115" s="34"/>
       <c r="H115" s="34"/>
@@ -5150,17 +5424,19 @@
       <c r="R115" s="21"/>
     </row>
     <row r="116" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="32" t="s">
+      <c r="A116" s="47" t="s">
         <v>325</v>
       </c>
-      <c r="B116" s="32"/>
-      <c r="C116" s="32" t="s">
+      <c r="B116" s="47"/>
+      <c r="C116" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="D116" s="34" t="s">
+      <c r="D116" s="48" t="s">
         <v>343</v>
       </c>
-      <c r="E116" s="34"/>
+      <c r="E116" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F116" s="34"/>
       <c r="G116" s="34"/>
       <c r="H116" s="34"/>
@@ -5176,17 +5452,19 @@
       <c r="R116" s="21"/>
     </row>
     <row r="117" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="32" t="s">
+      <c r="A117" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="B117" s="32"/>
-      <c r="C117" s="32" t="s">
+      <c r="B117" s="47"/>
+      <c r="C117" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="D117" s="32" t="s">
+      <c r="D117" s="47" t="s">
         <v>365</v>
       </c>
-      <c r="E117" s="34"/>
+      <c r="E117" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F117" s="34"/>
       <c r="G117" s="34"/>
       <c r="H117" s="34"/>
@@ -5204,17 +5482,19 @@
       <c r="R117" s="21"/>
     </row>
     <row r="118" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="32" t="s">
+      <c r="A118" s="47" t="s">
         <v>327</v>
       </c>
-      <c r="B118" s="32"/>
-      <c r="C118" s="32" t="s">
+      <c r="B118" s="47"/>
+      <c r="C118" s="47" t="s">
         <v>327</v>
       </c>
-      <c r="D118" s="34" t="s">
+      <c r="D118" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="E118" s="34"/>
+      <c r="E118" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F118" s="34"/>
       <c r="G118" s="34"/>
       <c r="H118" s="34"/>
@@ -5230,17 +5510,19 @@
       <c r="R118" s="21"/>
     </row>
     <row r="119" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="32" t="s">
+      <c r="A119" s="47" t="s">
         <v>328</v>
       </c>
-      <c r="B119" s="32"/>
-      <c r="C119" s="32" t="s">
+      <c r="B119" s="47"/>
+      <c r="C119" s="47" t="s">
         <v>328</v>
       </c>
-      <c r="D119" s="34" t="s">
+      <c r="D119" s="48" t="s">
         <v>345</v>
       </c>
-      <c r="E119" s="34"/>
+      <c r="E119" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F119" s="34"/>
       <c r="G119" s="34"/>
       <c r="H119" s="34"/>
@@ -5256,17 +5538,19 @@
       <c r="R119" s="21"/>
     </row>
     <row r="120" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="32" t="s">
+      <c r="A120" s="47" t="s">
         <v>329</v>
       </c>
-      <c r="B120" s="32"/>
-      <c r="C120" s="32" t="s">
+      <c r="B120" s="47"/>
+      <c r="C120" s="47" t="s">
         <v>329</v>
       </c>
-      <c r="D120" s="34" t="s">
+      <c r="D120" s="48" t="s">
         <v>346</v>
       </c>
-      <c r="E120" s="34"/>
+      <c r="E120" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F120" s="34"/>
       <c r="G120" s="34"/>
       <c r="H120" s="34"/>
@@ -5282,17 +5566,19 @@
       <c r="R120" s="21"/>
     </row>
     <row r="121" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="32" t="s">
+      <c r="A121" s="47" t="s">
         <v>330</v>
       </c>
-      <c r="B121" s="32"/>
-      <c r="C121" s="32" t="s">
+      <c r="B121" s="47"/>
+      <c r="C121" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="D121" s="34" t="s">
+      <c r="D121" s="48" t="s">
         <v>347</v>
       </c>
-      <c r="E121" s="34"/>
+      <c r="E121" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F121" s="34"/>
       <c r="G121" s="34"/>
       <c r="H121" s="34"/>
@@ -5310,17 +5596,19 @@
       <c r="R121" s="21"/>
     </row>
     <row r="122" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="32" t="s">
+      <c r="A122" s="47" t="s">
         <v>331</v>
       </c>
-      <c r="B122" s="32"/>
-      <c r="C122" s="32" t="s">
+      <c r="B122" s="47"/>
+      <c r="C122" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D122" s="34" t="s">
+      <c r="D122" s="48" t="s">
         <v>348</v>
       </c>
-      <c r="E122" s="34"/>
+      <c r="E122" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F122" s="34"/>
       <c r="G122" s="34"/>
       <c r="H122" s="34"/>
@@ -5336,17 +5624,19 @@
       <c r="R122" s="21"/>
     </row>
     <row r="123" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A123" s="32" t="s">
+      <c r="A123" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="B123" s="32"/>
-      <c r="C123" s="32" t="s">
+      <c r="B123" s="47"/>
+      <c r="C123" s="47" t="s">
         <v>356</v>
       </c>
-      <c r="D123" s="34" t="s">
+      <c r="D123" s="48" t="s">
         <v>358</v>
       </c>
-      <c r="E123" s="34"/>
+      <c r="E123" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F123" s="34"/>
       <c r="G123" s="34"/>
       <c r="H123" s="34"/>
@@ -5362,17 +5652,19 @@
       <c r="R123" s="21"/>
     </row>
     <row r="124" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A124" s="32" t="s">
+      <c r="A124" s="47" t="s">
         <v>332</v>
       </c>
-      <c r="B124" s="32"/>
-      <c r="C124" s="38" t="s">
+      <c r="B124" s="47"/>
+      <c r="C124" s="49" t="s">
         <v>353</v>
       </c>
-      <c r="D124" s="34" t="s">
+      <c r="D124" s="48" t="s">
         <v>349</v>
       </c>
-      <c r="E124" s="34"/>
+      <c r="E124" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F124" s="34"/>
       <c r="G124" s="34"/>
       <c r="H124" s="34"/>
@@ -5388,17 +5680,19 @@
       <c r="R124" s="21"/>
     </row>
     <row r="125" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A125" s="32" t="s">
+      <c r="A125" s="47" t="s">
         <v>333</v>
       </c>
-      <c r="B125" s="32"/>
-      <c r="C125" s="32" t="s">
+      <c r="B125" s="47"/>
+      <c r="C125" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D125" s="34" t="s">
+      <c r="D125" s="48" t="s">
         <v>350</v>
       </c>
-      <c r="E125" s="34"/>
+      <c r="E125" s="34" t="s">
+        <v>383</v>
+      </c>
       <c r="F125" s="34"/>
       <c r="G125" s="34"/>
       <c r="H125" s="34"/>
@@ -5415,7 +5709,7 @@
     </row>
     <row r="126" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="34"/>
-      <c r="B126" s="39"/>
+      <c r="B126" s="35"/>
       <c r="C126" s="34"/>
       <c r="D126" s="34"/>
       <c r="E126" s="34"/>
@@ -5464,15 +5758,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="102.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>